<commit_message>
add: eval MEM block trimming
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="146">
   <si>
     <t>origin PPL</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Throughput</t>
+  </si>
+  <si>
+    <t>speedup</t>
   </si>
   <si>
     <t>no prune</t>
@@ -3161,10 +3164,10 @@
       <c r="B2" s="33"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="3">
         <v>48.3</v>
@@ -3202,7 +3205,7 @@
         <v>100</v>
       </c>
       <c r="Q2" s="50" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" ht="17.6" hidden="1" spans="1:15">
@@ -3212,10 +3215,10 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F3" s="3">
         <v>45</v>
@@ -3252,15 +3255,15 @@
     </row>
     <row r="4" ht="17.6" hidden="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" s="3">
         <v>39.5</v>
@@ -3302,10 +3305,10 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F5" s="3">
         <v>40.3</v>
@@ -3348,13 +3351,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F6" s="5">
         <v>43.4</v>
@@ -3398,7 +3401,7 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3421,7 +3424,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>60</v>
@@ -3511,7 +3514,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
@@ -3556,13 +3559,13 @@
         <v>17</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F11" s="34">
         <v>38.1</v>
@@ -3606,7 +3609,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -3714,7 +3717,7 @@
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>60</v>
@@ -3804,7 +3807,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
@@ -3849,7 +3852,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>60</v>
@@ -3897,7 +3900,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5">
@@ -3939,7 +3942,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5">
@@ -4065,7 +4068,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>60</v>
@@ -4113,7 +4116,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5">
@@ -4197,7 +4200,7 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5">
@@ -4242,7 +4245,7 @@
         <v>17</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>60</v>
@@ -4290,7 +4293,7 @@
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7">
@@ -4417,7 +4420,7 @@
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>60</v>
@@ -4507,7 +4510,7 @@
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7">
@@ -4552,7 +4555,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D34" s="39" t="s">
         <v>60</v>
@@ -4600,7 +4603,7 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -4620,7 +4623,7 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5">
@@ -4703,7 +4706,7 @@
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>60</v>
@@ -4751,7 +4754,7 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5">
@@ -4814,7 +4817,7 @@
   <sheetData>
     <row r="1" s="15" customFormat="1" ht="17.6" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>56</v>
@@ -4850,10 +4853,10 @@
         <v>31</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" s="15" customFormat="1" ht="17.6" spans="1:14">
@@ -4862,10 +4865,10 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="3">
         <v>48.3</v>
@@ -4906,10 +4909,10 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="3">
         <v>45</v>
@@ -4986,14 +4989,14 @@
     </row>
     <row r="5" s="15" customFormat="1" ht="17.6" hidden="1" spans="1:14">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E5" s="3">
         <v>39.5</v>
@@ -5074,10 +5077,10 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E7" s="3">
         <v>40.3</v>
@@ -5200,7 +5203,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5">
@@ -5324,7 +5327,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7">
@@ -5448,7 +5451,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5">
@@ -5572,7 +5575,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7">
@@ -5674,7 +5677,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5">
@@ -5733,7 +5736,7 @@
   <sheetData>
     <row r="1" ht="17.6" spans="1:10">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>97</v>
@@ -5760,7 +5763,7 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" ht="17.6" spans="1:10">
@@ -5984,7 +5987,7 @@
   <sheetData>
     <row r="1" ht="17.6" spans="1:10">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>97</v>
@@ -6011,7 +6014,7 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" ht="17.6" spans="1:10">
@@ -6231,7 +6234,7 @@
   <sheetData>
     <row r="1" ht="17.6" spans="1:10">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>97</v>
@@ -6258,7 +6261,7 @@
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" ht="17.6" spans="1:10">
@@ -10806,17 +10809,17 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="S42" sqref="S42"/>
+      <selection pane="bottomLeft" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="15.3076923076923" customWidth="1"/>
     <col min="2" max="2" width="11.5769230769231" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="12.2788461538462" customWidth="1"/>
     <col min="4" max="4" width="30.2403846153846" customWidth="1"/>
@@ -10833,13 +10836,16 @@
     <col min="15" max="15" width="10.4134615384615" style="58" customWidth="1"/>
     <col min="16" max="16" width="14.4230769230769" customWidth="1"/>
     <col min="17" max="17" width="13.1634615384615" customWidth="1"/>
-    <col min="18" max="20" width="12.6923076923077" style="32"/>
+    <col min="18" max="18" width="12.6923076923077" style="32"/>
+    <col min="19" max="19" width="13.5288461538462" style="32" customWidth="1"/>
+    <col min="20" max="20" width="12.6923076923077" style="32"/>
     <col min="21" max="21" width="9.23076923076923" style="75"/>
     <col min="22" max="22" width="21.7115384615385" style="75" customWidth="1"/>
-    <col min="23" max="23" width="9.23076923076923" style="75"/>
+    <col min="23" max="23" width="14.7692307692308" style="75" customWidth="1"/>
+    <col min="24" max="24" width="12.9230769230769"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="1" ht="17.6" spans="1:23">
+    <row r="1" s="15" customFormat="1" ht="17.6" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -10908,6 +10914,9 @@
       </c>
       <c r="W1" s="81" t="s">
         <v>110</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="2" s="15" customFormat="1" ht="17.6" spans="1:23">
@@ -10917,10 +10926,10 @@
       <c r="B2" s="33"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="3">
         <v>48.3</v>
@@ -10955,7 +10964,7 @@
         <v>0.0124999999999957</v>
       </c>
       <c r="R2" s="50" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S2" s="50">
         <v>16375728128</v>
@@ -10978,7 +10987,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F3" s="3">
         <v>35</v>
@@ -11013,7 +11022,7 @@
         <v>-7.8875</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -11028,10 +11037,10 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" s="3">
         <v>45</v>
@@ -11121,15 +11130,15 @@
     </row>
     <row r="6" s="15" customFormat="1" ht="17.6" spans="1:23">
       <c r="A6" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F6" s="3">
         <v>39.5</v>
@@ -11224,10 +11233,10 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F8" s="3">
         <v>40.3</v>
@@ -11315,7 +11324,7 @@
       <c r="V9" s="82"/>
       <c r="W9" s="82"/>
     </row>
-    <row r="10" s="16" customFormat="1" ht="17.6" spans="1:23">
+    <row r="10" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A10" s="5" t="s">
         <v>47</v>
       </c>
@@ -11329,7 +11338,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F10" s="5">
         <v>43.4</v>
@@ -11363,16 +11372,32 @@
         <f>N10-61.6</f>
         <v>-2.41249999999999</v>
       </c>
-      <c r="U10" s="83"/>
-      <c r="V10" s="83"/>
-      <c r="W10" s="83"/>
+      <c r="S10" s="16">
+        <v>14714784320</v>
+      </c>
+      <c r="T10" s="16">
+        <v>28203</v>
+      </c>
+      <c r="U10" s="83">
+        <v>29403</v>
+      </c>
+      <c r="V10" s="83">
+        <v>0.4467</v>
+      </c>
+      <c r="W10" s="83">
+        <v>2.24</v>
+      </c>
+      <c r="X10" s="16">
+        <f>0.4884/V10</f>
+        <v>1.09335124244459</v>
+      </c>
     </row>
     <row r="11" s="16" customFormat="1" ht="17.6" spans="1:23">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -11392,7 +11417,7 @@
       <c r="V11" s="83"/>
       <c r="W11" s="83"/>
     </row>
-    <row r="12" s="16" customFormat="1" ht="17.6" spans="1:23">
+    <row r="12" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -11435,7 +11460,7 @@
         <v>-2.1375</v>
       </c>
       <c r="R12" s="51" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S12" s="51">
         <v>14870497802</v>
@@ -11451,6 +11476,10 @@
       </c>
       <c r="W12" s="83">
         <v>2.15</v>
+      </c>
+      <c r="X12" s="16">
+        <f>0.4884/V12</f>
+        <v>1.05077452667814</v>
       </c>
     </row>
     <row r="13" s="16" customFormat="1" ht="17.6" spans="1:23">
@@ -11505,7 +11534,7 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5">
@@ -11547,7 +11576,7 @@
       <c r="V14" s="83"/>
       <c r="W14" s="83"/>
     </row>
-    <row r="15" s="17" customFormat="1" ht="17.6" spans="1:23">
+    <row r="15" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A15" s="34" t="s">
         <v>50</v>
       </c>
@@ -11561,7 +11590,7 @@
         <v>60</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F15" s="34">
         <v>38.1</v>
@@ -11595,16 +11624,32 @@
         <f>N15-61.6</f>
         <v>-5.25</v>
       </c>
-      <c r="U15" s="84"/>
-      <c r="V15" s="84"/>
-      <c r="W15" s="84"/>
-    </row>
-    <row r="16" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="S15" s="17">
+        <v>13053840512</v>
+      </c>
+      <c r="T15" s="17">
+        <v>25035</v>
+      </c>
+      <c r="U15" s="84">
+        <v>26235</v>
+      </c>
+      <c r="V15" s="84">
+        <v>0.4155</v>
+      </c>
+      <c r="W15" s="84">
+        <v>2.41</v>
+      </c>
+      <c r="X15" s="16">
+        <f>0.4884/V15</f>
+        <v>1.17545126353791</v>
+      </c>
+    </row>
+    <row r="16" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -11623,8 +11668,9 @@
       <c r="U16" s="84"/>
       <c r="V16" s="84"/>
       <c r="W16" s="84"/>
-    </row>
-    <row r="17" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X16" s="16"/>
+    </row>
+    <row r="17" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -11667,7 +11713,7 @@
         <v>-7.00000000000001</v>
       </c>
       <c r="R17" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="S17" s="52">
         <v>13365267476</v>
@@ -11684,8 +11730,12 @@
       <c r="W17" s="84">
         <v>2.18</v>
       </c>
-    </row>
-    <row r="18" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X17" s="16">
+        <f>0.4884/V17</f>
+        <v>1.06428415776858</v>
+      </c>
+    </row>
+    <row r="18" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -11730,8 +11780,9 @@
       <c r="U18" s="84"/>
       <c r="V18" s="84"/>
       <c r="W18" s="84"/>
-    </row>
-    <row r="19" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X18" s="16"/>
+    </row>
+    <row r="19" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -11779,8 +11830,9 @@
       <c r="U19" s="84"/>
       <c r="V19" s="84"/>
       <c r="W19" s="84"/>
-    </row>
-    <row r="20" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X19" s="16"/>
+    </row>
+    <row r="20" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -11826,13 +11878,14 @@
       <c r="U20" s="84"/>
       <c r="V20" s="84"/>
       <c r="W20" s="84"/>
-    </row>
-    <row r="21" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X20" s="16"/>
+    </row>
+    <row r="21" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
@@ -11873,8 +11926,9 @@
       <c r="U21" s="84"/>
       <c r="V21" s="84"/>
       <c r="W21" s="84"/>
-    </row>
-    <row r="22" s="16" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X21" s="16"/>
+    </row>
+    <row r="22" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
@@ -11920,16 +11974,32 @@
         <f>N22-61.6</f>
         <v>-7.1</v>
       </c>
-      <c r="U22" s="83"/>
-      <c r="V22" s="83"/>
-      <c r="W22" s="83"/>
+      <c r="S22" s="16">
+        <v>11392896704</v>
+      </c>
+      <c r="T22" s="16">
+        <v>21868</v>
+      </c>
+      <c r="U22" s="83">
+        <v>23068</v>
+      </c>
+      <c r="V22" s="83">
+        <v>0.3722</v>
+      </c>
+      <c r="W22" s="83">
+        <v>2.69</v>
+      </c>
+      <c r="X22" s="16">
+        <f>0.4884/V22</f>
+        <v>1.31219774314884</v>
+      </c>
     </row>
     <row r="23" s="16" customFormat="1" ht="17.6" spans="1:23">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5">
@@ -11973,7 +12043,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5">
@@ -12015,7 +12085,7 @@
       <c r="V24" s="83"/>
       <c r="W24" s="83"/>
     </row>
-    <row r="25" s="16" customFormat="1" ht="17.6" spans="1:23">
+    <row r="25" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36" t="s">
@@ -12058,7 +12128,7 @@
         <v>-9.05</v>
       </c>
       <c r="R25" s="51" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="S25" s="51">
         <v>11860037150</v>
@@ -12074,6 +12144,10 @@
       </c>
       <c r="W25" s="83">
         <v>2.45</v>
+      </c>
+      <c r="X25" s="16">
+        <f>0.4884/V25</f>
+        <v>1.19735229222849</v>
       </c>
     </row>
     <row r="26" s="16" customFormat="1" ht="17.6" spans="1:23">
@@ -12176,7 +12250,7 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5">
@@ -12270,7 +12344,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5">
@@ -12312,7 +12386,7 @@
       <c r="V30" s="83"/>
       <c r="W30" s="83"/>
     </row>
-    <row r="31" s="17" customFormat="1" ht="17.6" spans="1:23">
+    <row r="31" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A31" s="7" t="s">
         <v>54</v>
       </c>
@@ -12358,16 +12432,32 @@
         <f>N31-61.6</f>
         <v>-9.7625</v>
       </c>
-      <c r="U31" s="84"/>
-      <c r="V31" s="84"/>
-      <c r="W31" s="84"/>
-    </row>
-    <row r="32" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="S31" s="17">
+        <v>9731952896</v>
+      </c>
+      <c r="T31" s="17">
+        <v>18700</v>
+      </c>
+      <c r="U31" s="84">
+        <v>19900</v>
+      </c>
+      <c r="V31" s="84">
+        <v>0.3417</v>
+      </c>
+      <c r="W31" s="84">
+        <v>2.93</v>
+      </c>
+      <c r="X31" s="16">
+        <f>0.4884/V31</f>
+        <v>1.42932396839333</v>
+      </c>
+    </row>
+    <row r="32" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7">
@@ -12408,8 +12498,9 @@
       <c r="U32" s="84"/>
       <c r="V32" s="84"/>
       <c r="W32" s="84"/>
-    </row>
-    <row r="33" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X32" s="16"/>
+    </row>
+    <row r="33" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A33" s="37"/>
       <c r="B33" s="37"/>
       <c r="C33" s="37" t="s">
@@ -12452,7 +12543,7 @@
         <v>-11.5375</v>
       </c>
       <c r="R33" s="52" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="S33" s="52">
         <v>10354806824</v>
@@ -12469,8 +12560,12 @@
       <c r="W33" s="84">
         <v>2.64</v>
       </c>
-    </row>
-    <row r="34" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X33" s="16">
+        <f>0.4884/V33</f>
+        <v>1.28763511732138</v>
+      </c>
+    </row>
+    <row r="34" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A34" s="38"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -12516,8 +12611,9 @@
       <c r="U34" s="84"/>
       <c r="V34" s="84"/>
       <c r="W34" s="84"/>
-    </row>
-    <row r="35" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X34" s="16"/>
+    </row>
+    <row r="35" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
@@ -12565,8 +12661,9 @@
       <c r="U35" s="84"/>
       <c r="V35" s="84"/>
       <c r="W35" s="84"/>
-    </row>
-    <row r="36" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X35" s="16"/>
+    </row>
+    <row r="36" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -12612,13 +12709,14 @@
       <c r="U36" s="84"/>
       <c r="V36" s="84"/>
       <c r="W36" s="84"/>
-    </row>
-    <row r="37" s="17" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X36" s="16"/>
+    </row>
+    <row r="37" s="17" customFormat="1" ht="17.6" spans="1:24">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
@@ -12659,8 +12757,9 @@
       <c r="U37" s="84"/>
       <c r="V37" s="84"/>
       <c r="W37" s="84"/>
-    </row>
-    <row r="38" s="16" customFormat="1" ht="17.6" spans="1:23">
+      <c r="X37" s="16"/>
+    </row>
+    <row r="38" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A38" s="39" t="s">
         <v>72</v>
       </c>
@@ -12707,14 +12806,24 @@
         <v>-13.4875</v>
       </c>
       <c r="R38" s="51"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="83"/>
+      <c r="S38" s="51">
+        <v>8071009088</v>
+      </c>
+      <c r="T38" s="51">
+        <v>15532</v>
+      </c>
+      <c r="U38" s="83">
+        <v>16732</v>
+      </c>
       <c r="V38" s="83">
-        <v>0.3012</v>
+        <v>0.2997</v>
       </c>
       <c r="W38" s="83">
-        <v>3.32</v>
+        <v>3.34</v>
+      </c>
+      <c r="X38" s="16">
+        <f>0.4884/V38</f>
+        <v>1.62962962962963</v>
       </c>
     </row>
     <row r="39" s="16" customFormat="1" ht="17.6" spans="1:23">
@@ -12722,7 +12831,7 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5">
@@ -12764,7 +12873,7 @@
       <c r="V39" s="83"/>
       <c r="W39" s="83"/>
     </row>
-    <row r="40" s="16" customFormat="1" ht="17.6" spans="1:23">
+    <row r="40" s="16" customFormat="1" ht="17.6" spans="1:24">
       <c r="A40" s="40"/>
       <c r="B40" s="40"/>
       <c r="C40" s="40" t="s">
@@ -12785,7 +12894,7 @@
       <c r="N40" s="10"/>
       <c r="O40" s="30"/>
       <c r="R40" s="51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="S40" s="51">
         <v>8849576498</v>
@@ -12801,6 +12910,10 @@
       </c>
       <c r="W40" s="83">
         <v>2.95</v>
+      </c>
+      <c r="X40" s="16">
+        <f>0.4884/V40</f>
+        <v>1.44198405668733</v>
       </c>
     </row>
     <row r="41" s="16" customFormat="1" ht="17.6" spans="1:23">
@@ -12882,7 +12995,7 @@
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5">
@@ -12950,7 +13063,7 @@
   <sheetData>
     <row r="1" s="53" customFormat="1" spans="1:11">
       <c r="A1" s="60" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" s="61" t="s">
         <v>2</v>
@@ -12980,13 +13093,13 @@
         <v>31</v>
       </c>
       <c r="K1" s="62" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" s="54" customFormat="1" spans="1:11">
       <c r="A2" s="63"/>
       <c r="B2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C2" s="3">
         <v>48.3</v>
@@ -13058,7 +13171,7 @@
         <v>0.908</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C4" s="68">
         <v>43.3</v>
@@ -13092,7 +13205,7 @@
     <row r="5" ht="17" customHeight="1" spans="1:11">
       <c r="A5" s="65"/>
       <c r="B5" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C5" s="68">
         <v>43.7</v>
@@ -13119,7 +13232,7 @@
         <v>68.6</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" s="55" customFormat="1" spans="1:11">
@@ -13163,7 +13276,7 @@
         <v>0.816</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C7" s="72">
         <v>38.4</v>
@@ -13197,7 +13310,7 @@
     <row r="8" s="55" customFormat="1" spans="1:11">
       <c r="A8" s="69"/>
       <c r="B8" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C8" s="72">
         <v>39.5</v>
@@ -13224,7 +13337,7 @@
         <v>68.4</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -13268,7 +13381,7 @@
         <v>0.724</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" s="68">
         <v>36.4</v>
@@ -13302,7 +13415,7 @@
     <row r="11" spans="1:11">
       <c r="A11" s="65"/>
       <c r="B11" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C11" s="68">
         <v>38.7</v>
@@ -13329,7 +13442,7 @@
         <v>66.5</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" s="55" customFormat="1" spans="1:11">
@@ -13373,7 +13486,7 @@
         <v>0.632</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C13" s="72">
         <v>31.7</v>
@@ -13407,7 +13520,7 @@
     <row r="14" s="55" customFormat="1" spans="1:11">
       <c r="A14" s="69"/>
       <c r="B14" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C14" s="72">
         <v>35.7</v>
@@ -13434,7 +13547,7 @@
         <v>64.6</v>
       </c>
       <c r="K14" s="72" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" s="56" customFormat="1" spans="1:11">
@@ -13478,7 +13591,7 @@
         <v>0.54</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C16" s="68">
         <v>31</v>
@@ -13512,7 +13625,7 @@
     <row r="17" s="56" customFormat="1" spans="1:11">
       <c r="A17" s="65"/>
       <c r="B17" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C17" s="68">
         <v>32.3</v>
@@ -13539,7 +13652,7 @@
         <v>62</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mod: mixtral expert to 1
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="8700" tabRatio="872" firstSheet="14" activeTab="23"/>
+    <workbookView windowWidth="25600" windowHeight="8700" tabRatio="872" firstSheet="15" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,9 @@
     <sheet name="finetune" sheetId="12" r:id="rId21"/>
     <sheet name="greedy_block" sheetId="16" r:id="rId22"/>
     <sheet name="active_cmp" sheetId="18" r:id="rId23"/>
-    <sheet name="mixtral" sheetId="24" r:id="rId24"/>
-    <sheet name="mixtral_block" sheetId="25" r:id="rId25"/>
+    <sheet name="mixtral_e2" sheetId="24" r:id="rId24"/>
+    <sheet name="mixtral_e1" sheetId="26" r:id="rId25"/>
+    <sheet name="mixtral_block" sheetId="25" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="178">
   <si>
     <t>origin PPL</t>
   </si>
@@ -12623,8 +12624,8 @@
   <sheetPr/>
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R9" sqref="A1:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -12637,6 +12638,7 @@
     <col min="14" max="14" width="7.36538461538461" customWidth="1"/>
     <col min="15" max="15" width="20.6730769230769" customWidth="1"/>
     <col min="16" max="16" width="13.4519230769231" customWidth="1"/>
+    <col min="17" max="17" width="12.9230769230769"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.6" spans="1:18">
@@ -12722,6 +12724,457 @@
       <c r="J2" s="11">
         <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
         <v>67.8833333333333</v>
+      </c>
+      <c r="K2" s="10">
+        <v>46702792704</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="10">
+        <v>45334</v>
+      </c>
+      <c r="N2" s="10">
+        <v>47951</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1.0751</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="Q2" s="19">
+        <f>P2/0.93</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="17.6" spans="1:17">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>56.3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>83.9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>62.6</v>
+      </c>
+      <c r="F3" s="5">
+        <v>46.8</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5">
+        <v>66.8</v>
+      </c>
+      <c r="I3" s="5">
+        <v>76.4</v>
+      </c>
+      <c r="J3" s="13">
+        <f t="shared" si="0"/>
+        <v>65.4666666666667</v>
+      </c>
+      <c r="K3" s="14">
+        <v>43531898934</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="14">
+        <v>45334.7</v>
+      </c>
+      <c r="N3" s="17">
+        <v>48026</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1.0204</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0.98</v>
+      </c>
+      <c r="Q3" s="19">
+        <f t="shared" ref="Q3:Q9" si="1">P3/0.93</f>
+        <v>1.05376344086022</v>
+      </c>
+    </row>
+    <row r="4" ht="17.6" spans="1:17">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6">
+        <v>55.4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>82.5</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
+        <v>56.6</v>
+      </c>
+      <c r="F4" s="6">
+        <v>45</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6">
+        <v>67.5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>74.2</v>
+      </c>
+      <c r="J4" s="15">
+        <f t="shared" si="0"/>
+        <v>63.5333333333333</v>
+      </c>
+      <c r="K4" s="16">
+        <v>40361005164</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N4" s="18">
+        <v>47813</v>
+      </c>
+      <c r="O4" s="18">
+        <v>0.9701</v>
+      </c>
+      <c r="P4" s="18">
+        <v>1.03</v>
+      </c>
+      <c r="Q4" s="19">
+        <f t="shared" si="1"/>
+        <v>1.10752688172043</v>
+      </c>
+    </row>
+    <row r="5" ht="17.6" spans="1:17">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>52</v>
+      </c>
+      <c r="C5" s="5">
+        <v>82.6</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
+        <v>53.4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>44.2</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>63.9</v>
+      </c>
+      <c r="I5" s="5">
+        <v>74.4</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="0"/>
+        <v>61.75</v>
+      </c>
+      <c r="K5" s="14">
+        <v>37190111394</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N5" s="17">
+        <v>47534</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0.9127</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1.1</v>
+      </c>
+      <c r="Q5" s="19">
+        <f t="shared" si="1"/>
+        <v>1.18279569892473</v>
+      </c>
+    </row>
+    <row r="6" ht="17.6" spans="1:17">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7">
+        <v>48.6</v>
+      </c>
+      <c r="C6" s="7">
+        <v>83</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>49.2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>44.4</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
+        <v>65.3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>72.9</v>
+      </c>
+      <c r="J6" s="15">
+        <f t="shared" si="0"/>
+        <v>60.5666666666667</v>
+      </c>
+      <c r="K6" s="16">
+        <v>34019217624</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N6" s="18">
+        <v>47405</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0.8694</v>
+      </c>
+      <c r="P6" s="18">
+        <v>1.15</v>
+      </c>
+      <c r="Q6" s="19">
+        <f t="shared" si="1"/>
+        <v>1.23655913978495</v>
+      </c>
+    </row>
+    <row r="7" ht="17.6" spans="1:17">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8">
+        <v>47.1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>82.2</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <v>43.5</v>
+      </c>
+      <c r="F7" s="8">
+        <v>41.6</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8">
+        <v>61.7</v>
+      </c>
+      <c r="I7" s="8">
+        <v>73.7</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" si="0"/>
+        <v>58.3</v>
+      </c>
+      <c r="K7" s="17">
+        <v>30848323854</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="17">
+        <v>45334</v>
+      </c>
+      <c r="N7" s="17">
+        <v>47220</v>
+      </c>
+      <c r="O7" s="17">
+        <v>0.8211</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1.22</v>
+      </c>
+      <c r="Q7" s="19">
+        <f t="shared" si="1"/>
+        <v>1.31182795698925</v>
+      </c>
+    </row>
+    <row r="8" ht="17.6" spans="1:17">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>42.5</v>
+      </c>
+      <c r="C8">
+        <v>77.7</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>41.4</v>
+      </c>
+      <c r="H8">
+        <v>56.3</v>
+      </c>
+      <c r="I8">
+        <v>69.3</v>
+      </c>
+      <c r="J8" s="13">
+        <f>AVERAGE(B8:I8)</f>
+        <v>52.8666666666667</v>
+      </c>
+      <c r="K8">
+        <v>27677430084</v>
+      </c>
+      <c r="M8" s="17">
+        <v>45335</v>
+      </c>
+      <c r="N8">
+        <v>47187</v>
+      </c>
+      <c r="O8">
+        <v>0.7816</v>
+      </c>
+      <c r="P8">
+        <v>1.28</v>
+      </c>
+      <c r="Q8" s="19">
+        <f t="shared" si="1"/>
+        <v>1.37634408602151</v>
+      </c>
+    </row>
+    <row r="9" ht="17.6" spans="1:17">
+      <c r="A9">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>41.6</v>
+      </c>
+      <c r="C9">
+        <v>74.5</v>
+      </c>
+      <c r="E9">
+        <v>27.7</v>
+      </c>
+      <c r="F9">
+        <v>39.6</v>
+      </c>
+      <c r="H9">
+        <v>54.2</v>
+      </c>
+      <c r="I9">
+        <v>70.4</v>
+      </c>
+      <c r="J9" s="13">
+        <f>AVERAGE(B9:I9)</f>
+        <v>51.3333333333333</v>
+      </c>
+      <c r="K9">
+        <v>24506536314</v>
+      </c>
+      <c r="M9">
+        <v>45334</v>
+      </c>
+      <c r="N9">
+        <v>47240</v>
+      </c>
+      <c r="O9">
+        <v>0.7377</v>
+      </c>
+      <c r="P9">
+        <v>1.36</v>
+      </c>
+      <c r="Q9" s="19">
+        <f t="shared" si="1"/>
+        <v>1.46236559139785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <cols>
+    <col min="11" max="11" width="17.2980769230769" customWidth="1"/>
+    <col min="12" max="12" width="9.93269230769231" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.6" spans="1:18">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" ht="17.6" spans="1:17">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="11" t="e">
+        <f t="shared" ref="J2:J9" si="0">AVERAGE(B2:I2)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="12"/>
@@ -12735,29 +13188,17 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
-        <v>56.3</v>
-      </c>
-      <c r="C3" s="5">
-        <v>83.9</v>
-      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5">
-        <v>62.6</v>
-      </c>
-      <c r="F3" s="5">
-        <v>46.8</v>
-      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="5">
-        <v>66.8</v>
-      </c>
-      <c r="I3" s="5">
-        <v>76.4</v>
-      </c>
-      <c r="J3" s="13">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>65.4666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="12"/>
@@ -12771,29 +13212,17 @@
       <c r="A4">
         <v>6</v>
       </c>
-      <c r="B4" s="6">
-        <v>55.4</v>
-      </c>
-      <c r="C4" s="6">
-        <v>82.5</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6">
-        <v>56.6</v>
-      </c>
-      <c r="F4" s="6">
-        <v>45</v>
-      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6">
-        <v>67.5</v>
-      </c>
-      <c r="I4" s="6">
-        <v>74.2</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="15" t="e">
         <f t="shared" si="0"/>
-        <v>63.5333333333333</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="12"/>
@@ -12807,33 +13236,21 @@
       <c r="A5">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
-        <v>52</v>
-      </c>
-      <c r="C5" s="5">
-        <v>82.6</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5">
-        <v>53.4</v>
-      </c>
-      <c r="F5" s="5">
-        <v>44.2</v>
-      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="5">
-        <v>63.9</v>
-      </c>
-      <c r="I5" s="5">
-        <v>74.4</v>
-      </c>
-      <c r="J5" s="13">
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>61.75</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="14"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
@@ -12843,29 +13260,17 @@
       <c r="A6">
         <v>12</v>
       </c>
-      <c r="B6" s="7">
-        <v>48.6</v>
-      </c>
-      <c r="C6" s="7">
-        <v>83</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7">
-        <v>49.2</v>
-      </c>
-      <c r="F6" s="7">
-        <v>44.4</v>
-      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7">
-        <v>65.3</v>
-      </c>
-      <c r="I6" s="7">
-        <v>72.9</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="15" t="e">
         <f t="shared" si="0"/>
-        <v>60.5666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="12"/>
@@ -12879,29 +13284,17 @@
       <c r="A7">
         <v>15</v>
       </c>
-      <c r="B7" s="8">
-        <v>47.1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>82.2</v>
-      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="8">
-        <v>43.5</v>
-      </c>
-      <c r="F7" s="8">
-        <v>41.6</v>
-      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="8">
-        <v>61.7</v>
-      </c>
-      <c r="I7" s="8">
-        <v>73.7</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>58.3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="12"/>
@@ -12909,76 +13302,35 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="14"/>
-    </row>
-    <row r="8" ht="17.6" spans="1:10">
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" ht="17.6" spans="1:17">
       <c r="A8">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>42.5</v>
-      </c>
-      <c r="C8">
-        <v>77.7</v>
-      </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>41.4</v>
-      </c>
-      <c r="H8">
-        <v>56.3</v>
-      </c>
-      <c r="I8">
-        <v>69.3</v>
-      </c>
-      <c r="J8" s="13">
-        <f>AVERAGE(B8:I8)</f>
-        <v>52.8666666666667</v>
-      </c>
-    </row>
-    <row r="9" ht="17.6" spans="1:16">
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="J8" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8" s="19"/>
+    </row>
+    <row r="9" ht="17.6" spans="1:17">
       <c r="A9">
         <v>21</v>
       </c>
-      <c r="B9">
-        <v>41.6</v>
-      </c>
-      <c r="C9">
-        <v>74.5</v>
-      </c>
-      <c r="E9">
-        <v>27.7</v>
-      </c>
-      <c r="F9">
-        <v>39.6</v>
-      </c>
-      <c r="H9">
-        <v>54.2</v>
-      </c>
-      <c r="I9">
-        <v>70.4</v>
-      </c>
-      <c r="J9" s="13">
-        <f>AVERAGE(B9:I9)</f>
-        <v>51.3333333333333</v>
-      </c>
-      <c r="K9">
-        <v>39304040574</v>
-      </c>
-      <c r="M9">
-        <v>45334</v>
-      </c>
-      <c r="N9">
-        <v>47239</v>
-      </c>
-      <c r="O9">
-        <v>0.7606</v>
-      </c>
-      <c r="P9">
-        <v>1.31</v>
-      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="J9" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12986,7 +13338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:R16"/>

</xml_diff>

<commit_message>
add: hyper exp for deepseek
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9100" tabRatio="872" firstSheet="18" activeTab="27"/>
+    <workbookView windowWidth="25600" windowHeight="9100" tabRatio="872" firstSheet="18" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12624,15 +12624,16 @@
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="11" max="11" width="15.0576923076923" customWidth="1"/>
+    <col min="17" max="17" width="12.9230769230769"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.6" spans="1:18">
@@ -12717,13 +12718,26 @@
         <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
         <v>67.5833333333333</v>
       </c>
-      <c r="K2" s="10"/>
+      <c r="K2" s="10">
+        <v>46702792704</v>
+      </c>
       <c r="L2" s="12"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="19"/>
+      <c r="M2" s="10">
+        <v>45334</v>
+      </c>
+      <c r="N2" s="10">
+        <v>47951</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1.0751</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="Q2" s="19">
+        <f>P2/0.93</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="17.6" spans="1:17">
       <c r="A3">
@@ -12751,13 +12765,26 @@
         <f t="shared" si="0"/>
         <v>66.7166666666667</v>
       </c>
-      <c r="K3" s="14"/>
+      <c r="K3" s="14">
+        <v>42348982272</v>
+      </c>
       <c r="L3" s="12"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="19"/>
+      <c r="M3" s="14">
+        <v>45334</v>
+      </c>
+      <c r="N3" s="17">
+        <v>42659</v>
+      </c>
+      <c r="O3" s="17">
+        <v>1.0515</v>
+      </c>
+      <c r="P3" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="Q3" s="19">
+        <f>P3/0.93</f>
+        <v>1.02150537634409</v>
+      </c>
     </row>
     <row r="4" ht="17.6" spans="1:17">
       <c r="A4">
@@ -12785,13 +12812,26 @@
         <f t="shared" si="0"/>
         <v>63.2333333333333</v>
       </c>
-      <c r="K4" s="16"/>
+      <c r="K4" s="16">
+        <v>37995171840</v>
+      </c>
       <c r="L4" s="12"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="19"/>
+      <c r="M4" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N4" s="18">
+        <v>37993</v>
+      </c>
+      <c r="O4" s="18">
+        <v>0.8639</v>
+      </c>
+      <c r="P4" s="18">
+        <v>1.16</v>
+      </c>
+      <c r="Q4" s="19">
+        <f>P4/0.93</f>
+        <v>1.24731182795699</v>
+      </c>
     </row>
     <row r="5" ht="17.6" spans="1:17">
       <c r="A5">
@@ -12819,13 +12859,26 @@
         <f t="shared" si="0"/>
         <v>57.4666666666667</v>
       </c>
-      <c r="K5" s="14"/>
+      <c r="K5" s="14">
+        <v>33641361408</v>
+      </c>
       <c r="L5" s="12"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="19"/>
+      <c r="M5" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N5" s="17">
+        <v>33557</v>
+      </c>
+      <c r="O5" s="17">
+        <v>0.7652</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1.31</v>
+      </c>
+      <c r="Q5" s="19">
+        <f>P5/0.93</f>
+        <v>1.40860215053763</v>
+      </c>
     </row>
     <row r="6" ht="17.6" spans="1:17">
       <c r="A6">
@@ -12853,13 +12906,26 @@
         <f t="shared" si="0"/>
         <v>45.4166666666667</v>
       </c>
-      <c r="K6" s="16"/>
+      <c r="K6" s="16">
+        <v>29287550976</v>
+      </c>
       <c r="L6" s="12"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="19"/>
+      <c r="M6" s="16">
+        <v>45334</v>
+      </c>
+      <c r="N6" s="18">
+        <v>29183</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0.616</v>
+      </c>
+      <c r="P6" s="18">
+        <v>1.62</v>
+      </c>
+      <c r="Q6" s="19">
+        <f>P6/0.93</f>
+        <v>1.74193548387097</v>
+      </c>
     </row>
     <row r="7" ht="17.6" spans="1:17">
       <c r="A7">
@@ -12887,13 +12953,36 @@
         <f t="shared" si="0"/>
         <v>38.7166666666667</v>
       </c>
-      <c r="K7" s="17"/>
+      <c r="K7" s="17">
+        <v>24933740544</v>
+      </c>
       <c r="L7" s="12"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="14"/>
+      <c r="M7" s="17">
+        <v>45334</v>
+      </c>
+      <c r="N7" s="17">
+        <v>24838</v>
+      </c>
+      <c r="O7" s="17">
+        <v>0.504</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1.98</v>
+      </c>
+      <c r="Q7" s="19">
+        <f>P7/0.93</f>
+        <v>2.12903225806452</v>
+      </c>
+    </row>
+    <row r="8" spans="13:13">
+      <c r="M8" s="17">
+        <v>45335</v>
+      </c>
+    </row>
+    <row r="9" spans="13:13">
+      <c r="M9">
+        <v>45334</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13061,7 +13150,7 @@
       </c>
       <c r="L3" s="12"/>
       <c r="M3" s="14">
-        <v>45334.7</v>
+        <v>45334</v>
       </c>
       <c r="N3" s="17">
         <v>48026</v>
@@ -13377,7 +13466,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L6" sqref="L6:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -14113,7 +14202,7 @@
   <sheetPr/>
   <dimension ref="D2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add: eval through block
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9520" tabRatio="872" firstSheet="28" activeTab="37"/>
+    <workbookView windowWidth="25600" windowHeight="9520" tabRatio="872" firstSheet="28" activeTab="35"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18358,7 +18358,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
@@ -18423,7 +18423,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18455,8 +18455,31 @@
         <f>AVERAGE(B2:I2)</f>
         <v>65.5125</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>14315784192</v>
+      </c>
+      <c r="L2">
+        <v>27420</v>
+      </c>
+      <c r="M2">
+        <v>28964</v>
+      </c>
+      <c r="N2">
+        <f>L2/27420</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0.5353</v>
+      </c>
+      <c r="P2">
+        <v>1.87</v>
+      </c>
+      <c r="Q2">
+        <f>P2/1.87</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>3</v>
       </c>
@@ -18488,8 +18511,31 @@
         <f>AVERAGE(B3:I3)</f>
         <v>63.85</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>12862458360</v>
+      </c>
+      <c r="L3">
+        <v>24646</v>
+      </c>
+      <c r="M3">
+        <v>26190</v>
+      </c>
+      <c r="N3">
+        <f>L3/27420</f>
+        <v>0.898832968636032</v>
+      </c>
+      <c r="O3">
+        <v>0.5026</v>
+      </c>
+      <c r="P3">
+        <v>1.99</v>
+      </c>
+      <c r="Q3">
+        <f>P3/1.87</f>
+        <v>1.06417112299465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>6</v>
       </c>
@@ -18521,8 +18567,31 @@
         <f>AVERAGE(B4:I4)</f>
         <v>62.4375</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>11409132528</v>
+      </c>
+      <c r="L4">
+        <v>21872</v>
+      </c>
+      <c r="M4">
+        <v>23437</v>
+      </c>
+      <c r="N4">
+        <f>L4/27420</f>
+        <v>0.797665937272064</v>
+      </c>
+      <c r="O4">
+        <v>0.4497</v>
+      </c>
+      <c r="P4">
+        <v>2.22</v>
+      </c>
+      <c r="Q4">
+        <f>P4/1.87</f>
+        <v>1.18716577540107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>9</v>
       </c>
@@ -18554,8 +18623,31 @@
         <f>AVERAGE(B5:I5)</f>
         <v>60.1875</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>9955806696</v>
+      </c>
+      <c r="L5">
+        <v>19097</v>
+      </c>
+      <c r="M5">
+        <v>20656</v>
+      </c>
+      <c r="N5">
+        <f>L5/27420</f>
+        <v>0.696462436177972</v>
+      </c>
+      <c r="O5">
+        <v>0.4109</v>
+      </c>
+      <c r="P5">
+        <v>2.43</v>
+      </c>
+      <c r="Q5">
+        <f>P5/1.87</f>
+        <v>1.29946524064171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>12</v>
       </c>
@@ -18587,8 +18679,31 @@
         <f>AVERAGE(B6:I6)</f>
         <v>56.3625</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>8502480864</v>
+      </c>
+      <c r="L6">
+        <v>16325</v>
+      </c>
+      <c r="M6">
+        <v>17877</v>
+      </c>
+      <c r="N6">
+        <f>L6/27420</f>
+        <v>0.595368344274252</v>
+      </c>
+      <c r="O6">
+        <v>0.3324</v>
+      </c>
+      <c r="P6">
+        <v>3.01</v>
+      </c>
+      <c r="Q6">
+        <f>P6/1.87</f>
+        <v>1.6096256684492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>15</v>
       </c>
@@ -18619,6 +18734,29 @@
       <c r="J7">
         <f>AVERAGE(B7:I7)</f>
         <v>54.0875</v>
+      </c>
+      <c r="K7">
+        <v>7049155032</v>
+      </c>
+      <c r="L7">
+        <v>13552</v>
+      </c>
+      <c r="M7">
+        <v>15102</v>
+      </c>
+      <c r="N7">
+        <f>L7/27420</f>
+        <v>0.494237782640408</v>
+      </c>
+      <c r="O7">
+        <v>0.294</v>
+      </c>
+      <c r="P7">
+        <v>3.4</v>
+      </c>
+      <c r="Q7">
+        <f>P7/1.87</f>
+        <v>1.81818181818182</v>
       </c>
     </row>
   </sheetData>
@@ -18632,11 +18770,16 @@
   <sheetPr/>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <cols>
+    <col min="11" max="11" width="13.6153846153846" customWidth="1"/>
+    <col min="14" max="14" width="12.9230769230769"/>
+    <col min="17" max="17" width="12.9230769230769"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -18691,7 +18834,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18723,8 +18866,31 @@
         <f>AVERAGE(B2:I2)</f>
         <v>65.5125</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>14315784192</v>
+      </c>
+      <c r="L2">
+        <v>27420</v>
+      </c>
+      <c r="M2">
+        <v>28964</v>
+      </c>
+      <c r="N2">
+        <f>L2/27420</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0.5353</v>
+      </c>
+      <c r="P2">
+        <v>1.87</v>
+      </c>
+      <c r="Q2">
+        <f>P2/1.87</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>3</v>
       </c>
@@ -18756,8 +18922,31 @@
         <f>AVERAGE(B3:I3)</f>
         <v>63.15</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>12758649372</v>
+      </c>
+      <c r="L3">
+        <v>24448</v>
+      </c>
+      <c r="M3">
+        <v>25992</v>
+      </c>
+      <c r="N3">
+        <f>L3/27420</f>
+        <v>0.891611962071481</v>
+      </c>
+      <c r="O3">
+        <v>0.4892</v>
+      </c>
+      <c r="P3">
+        <v>2.04</v>
+      </c>
+      <c r="Q3">
+        <f>P3/1.87</f>
+        <v>1.09090909090909</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>6</v>
       </c>
@@ -18789,8 +18978,31 @@
         <f>AVERAGE(B4:I4)</f>
         <v>62.625</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>11201514552</v>
+      </c>
+      <c r="L4">
+        <v>21476</v>
+      </c>
+      <c r="M4">
+        <v>23039</v>
+      </c>
+      <c r="N4">
+        <f>L4/27420</f>
+        <v>0.783223924142961</v>
+      </c>
+      <c r="O4">
+        <v>0.4381</v>
+      </c>
+      <c r="P4">
+        <v>2.28</v>
+      </c>
+      <c r="Q4">
+        <f>P4/1.87</f>
+        <v>1.2192513368984</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>9</v>
       </c>
@@ -18822,8 +19034,31 @@
         <f>AVERAGE(B5:I5)</f>
         <v>60.1375</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>9644379732</v>
+      </c>
+      <c r="L5">
+        <v>18505</v>
+      </c>
+      <c r="M5">
+        <v>20071</v>
+      </c>
+      <c r="N5">
+        <f>L5/27420</f>
+        <v>0.674872355944566</v>
+      </c>
+      <c r="O5">
+        <v>0.3923</v>
+      </c>
+      <c r="P5">
+        <v>2.55</v>
+      </c>
+      <c r="Q5">
+        <f>P5/1.87</f>
+        <v>1.36363636363636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>12</v>
       </c>
@@ -18855,8 +19090,31 @@
         <f>AVERAGE(B6:I6)</f>
         <v>57.35</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>8087244912</v>
+      </c>
+      <c r="L6">
+        <v>15533</v>
+      </c>
+      <c r="M6">
+        <v>17097</v>
+      </c>
+      <c r="N6">
+        <f>L6/27420</f>
+        <v>0.566484318016047</v>
+      </c>
+      <c r="O6">
+        <v>0.3474</v>
+      </c>
+      <c r="P6">
+        <v>2.88</v>
+      </c>
+      <c r="Q6">
+        <f>P6/1.87</f>
+        <v>1.54010695187166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>15</v>
       </c>
@@ -18887,6 +19145,29 @@
       <c r="J7">
         <f>AVERAGE(B7:I7)</f>
         <v>52.1625</v>
+      </c>
+      <c r="K7">
+        <v>6530110092</v>
+      </c>
+      <c r="L7">
+        <v>12561</v>
+      </c>
+      <c r="M7">
+        <v>14124</v>
+      </c>
+      <c r="N7">
+        <f>L7/27420</f>
+        <v>0.458096280087527</v>
+      </c>
+      <c r="O7">
+        <v>0.2795</v>
+      </c>
+      <c r="P7">
+        <v>3.58</v>
+      </c>
+      <c r="Q7">
+        <f>P7/1.87</f>
+        <v>1.9144385026738</v>
       </c>
     </row>
   </sheetData>
@@ -18901,7 +19182,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="A1:Q7"/>
+      <selection activeCell="K2" sqref="K2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
@@ -18959,7 +19240,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
@@ -18990,6 +19271,21 @@
       <c r="J2">
         <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
         <v>65.5125</v>
+      </c>
+      <c r="K2">
+        <v>14315784192</v>
+      </c>
+      <c r="L2">
+        <v>27420</v>
+      </c>
+      <c r="M2">
+        <v>28964</v>
+      </c>
+      <c r="O2">
+        <v>0.5353</v>
+      </c>
+      <c r="P2">
+        <v>1.87</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -19168,11 +19464,16 @@
   <sheetPr/>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <cols>
+    <col min="11" max="11" width="11.6923076923077" customWidth="1"/>
+    <col min="14" max="14" width="12.9230769230769"/>
+    <col min="17" max="17" width="12.9230769230769"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -19227,7 +19528,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -19259,170 +19560,308 @@
         <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
         <v>65.5125</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>14315784192</v>
+      </c>
+      <c r="L2">
+        <v>27420</v>
+      </c>
+      <c r="M2">
+        <v>28964</v>
+      </c>
+      <c r="N2">
+        <f>L2/27420</f>
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0.5353</v>
+      </c>
+      <c r="P2">
+        <v>1.87</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q7" si="1">P2/1.87</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>36.9</v>
+        <v>38.4</v>
       </c>
       <c r="C3">
-        <v>62.7</v>
+        <v>63.4</v>
       </c>
       <c r="D3">
-        <v>69.8</v>
+        <v>70.6</v>
       </c>
       <c r="E3">
-        <v>60.3</v>
+        <v>61</v>
       </c>
       <c r="F3">
-        <v>34.8</v>
+        <v>36.4</v>
       </c>
       <c r="G3" s="1">
-        <v>75.6</v>
+        <v>76.1</v>
       </c>
       <c r="H3">
-        <v>63.2</v>
+        <v>63.9</v>
       </c>
       <c r="I3">
-        <v>67.7</v>
+        <v>68.8</v>
       </c>
       <c r="J3">
         <f t="shared" si="0"/>
-        <v>58.875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>59.825</v>
+      </c>
+      <c r="K3">
+        <v>12758649372</v>
+      </c>
+      <c r="L3">
+        <v>24449</v>
+      </c>
+      <c r="M3">
+        <v>25993</v>
+      </c>
+      <c r="N3">
+        <f>L3/27420</f>
+        <v>0.891648431801605</v>
+      </c>
+      <c r="O3">
+        <v>0.488</v>
+      </c>
+      <c r="P3">
+        <v>2.05</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>1.09625668449198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>31.3</v>
+        <v>34.4</v>
       </c>
       <c r="C4">
-        <v>62.2</v>
+        <v>62.6</v>
       </c>
       <c r="D4">
-        <v>57.4</v>
+        <v>63.1</v>
       </c>
       <c r="E4">
-        <v>38.4</v>
+        <v>45.4</v>
       </c>
       <c r="F4">
-        <v>32</v>
+        <v>32.8</v>
       </c>
       <c r="G4">
-        <v>70.7</v>
+        <v>73.6</v>
       </c>
       <c r="H4">
-        <v>52.7</v>
+        <v>54.5</v>
       </c>
       <c r="I4">
-        <v>58.2</v>
+        <v>62.6</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>50.3625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>53.625</v>
+      </c>
+      <c r="K4">
+        <v>11201514552</v>
+      </c>
+      <c r="L4">
+        <v>21478</v>
+      </c>
+      <c r="M4">
+        <v>20322</v>
+      </c>
+      <c r="N4">
+        <f>L4/27420</f>
+        <v>0.783296863603209</v>
+      </c>
+      <c r="O4">
+        <v>0.4343</v>
+      </c>
+      <c r="P4">
+        <v>2.3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>1.22994652406417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>28</v>
+        <v>30.4</v>
       </c>
       <c r="C5">
-        <v>63.7</v>
+        <v>62.9</v>
       </c>
       <c r="D5">
-        <v>34.1</v>
+        <v>47.8</v>
       </c>
       <c r="E5">
-        <v>23.1</v>
+        <v>30.6</v>
       </c>
       <c r="F5">
-        <v>27.6</v>
+        <v>29.4</v>
       </c>
       <c r="G5">
-        <v>57.7</v>
+        <v>65.3</v>
       </c>
       <c r="H5">
-        <v>52.4</v>
+        <v>53.4</v>
       </c>
       <c r="I5">
-        <v>50.5</v>
+        <v>57.6</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>42.1375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>47.175</v>
+      </c>
+      <c r="K5">
+        <v>9644379732</v>
+      </c>
+      <c r="L5">
+        <v>18507</v>
+      </c>
+      <c r="M5">
+        <v>20051</v>
+      </c>
+      <c r="N5">
+        <f>L5/27420</f>
+        <v>0.674945295404814</v>
+      </c>
+      <c r="O5">
+        <v>0.3834</v>
+      </c>
+      <c r="P5">
+        <v>2.61</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>1.39572192513369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>27.9</v>
+        <v>28.8</v>
       </c>
       <c r="C6">
-        <v>42.6</v>
+        <v>55.2</v>
       </c>
       <c r="D6">
-        <v>27.2</v>
+        <v>36.4</v>
       </c>
       <c r="E6">
-        <v>22.9</v>
+        <v>23.5</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>27.6</v>
       </c>
       <c r="G6">
-        <v>53.4</v>
+        <v>60.8</v>
       </c>
       <c r="H6">
         <v>52.7</v>
       </c>
       <c r="I6">
-        <v>49.2</v>
+        <v>52.3</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>38.2375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>42.1625</v>
+      </c>
+      <c r="K6">
+        <v>8087244912</v>
+      </c>
+      <c r="L6">
+        <v>15534</v>
+      </c>
+      <c r="M6">
+        <v>17078</v>
+      </c>
+      <c r="N6">
+        <f>L6/27420</f>
+        <v>0.566520787746171</v>
+      </c>
+      <c r="O6">
+        <v>0.3304</v>
+      </c>
+      <c r="P6">
+        <v>3.03</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>1.62032085561497</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>26.8</v>
+        <v>25.2</v>
       </c>
       <c r="C7">
-        <v>53.2</v>
+        <v>38.6</v>
       </c>
       <c r="D7">
-        <v>24.6</v>
+        <v>30.2</v>
       </c>
       <c r="E7">
-        <v>24.5</v>
+        <v>23.1</v>
       </c>
       <c r="F7">
-        <v>29.2</v>
+        <v>27.2</v>
       </c>
       <c r="G7">
-        <v>48.8</v>
+        <v>54.8</v>
       </c>
       <c r="H7">
-        <v>48.8</v>
+        <v>51.6</v>
       </c>
       <c r="I7">
-        <v>52.4</v>
+        <v>49.8</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>38.5375</v>
+        <v>37.5625</v>
+      </c>
+      <c r="K7">
+        <v>6530110092</v>
+      </c>
+      <c r="L7">
+        <v>12562</v>
+      </c>
+      <c r="M7">
+        <v>14106</v>
+      </c>
+      <c r="N7">
+        <f>L7/27420</f>
+        <v>0.458132749817651</v>
+      </c>
+      <c r="O7">
+        <v>0.2745</v>
+      </c>
+      <c r="P7">
+        <v>3.64</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>1.94652406417112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: prune per layer model
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9520" tabRatio="872" firstSheet="9" activeTab="10"/>
+    <workbookView windowWidth="25600" windowHeight="9500" tabRatio="872" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,9 @@
     <sheet name="shared_e1" sheetId="22" state="hidden" r:id="rId20"/>
     <sheet name="shared_e2" sheetId="23" state="hidden" r:id="rId21"/>
     <sheet name="shared_e6" sheetId="21" r:id="rId22"/>
-    <sheet name="shared_e6_v2" sheetId="30" r:id="rId23"/>
+    <sheet name="shared_e6_ft" sheetId="12" r:id="rId23"/>
     <sheet name="shared_e6_ft_sft" sheetId="33" r:id="rId24"/>
-    <sheet name="shared_e6_ft" sheetId="12" r:id="rId25"/>
+    <sheet name="shared_e6_v2" sheetId="30" r:id="rId25"/>
     <sheet name="shared_e6_sft" sheetId="32" r:id="rId26"/>
     <sheet name="greedy_greedy_old" sheetId="13" state="hidden" r:id="rId27"/>
     <sheet name="greedy_block" sheetId="16" r:id="rId28"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="191">
   <si>
     <t>origin PPL</t>
   </si>
@@ -4003,7 +4003,7 @@
   <sheetPr/>
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="O61" sqref="O61"/>
@@ -9462,7 +9462,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I6"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -10556,7 +10556,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="A1:P7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
@@ -10934,23 +10934,23 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11:T12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
   <cols>
     <col min="4" max="4" width="12.6538461538462" customWidth="1"/>
-    <col min="7" max="7" width="14.7307692307692" customWidth="1"/>
-    <col min="8" max="8" width="10.1538461538462"/>
-    <col min="9" max="9" width="12.9230769230769"/>
-    <col min="10" max="10" width="10"/>
-    <col min="15" max="15" width="12.9230769230769"/>
+    <col min="8" max="8" width="14.7307692307692" customWidth="1"/>
+    <col min="9" max="9" width="10.1538461538462"/>
+    <col min="10" max="10" width="12.9230769230769"/>
+    <col min="11" max="11" width="10"/>
+    <col min="16" max="16" width="12.9230769230769"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.6" spans="1:16">
+    <row r="1" ht="17.6" spans="1:17">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -10964,43 +10964,46 @@
         <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="J1" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="2" ht="17.6" spans="1:16">
+    <row r="2" ht="17.6" spans="1:17">
       <c r="A2">
         <v>0</v>
       </c>
@@ -11014,45 +11017,48 @@
         <v>77.4</v>
       </c>
       <c r="E2" s="6">
+        <v>38.3</v>
+      </c>
+      <c r="F2" s="6">
         <v>44.2</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>78.7</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>70.1</v>
       </c>
-      <c r="H2" s="3">
-        <f t="shared" ref="H2:H7" si="0">AVERAGE(B2:G2)</f>
-        <v>65.2333333333333</v>
-      </c>
-      <c r="I2" s="24">
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I7" si="0">AVERAGE(B2:H2)</f>
+        <v>61.3857142857143</v>
+      </c>
+      <c r="J2" s="24">
         <v>16375728128</v>
       </c>
-      <c r="J2" s="25">
+      <c r="K2" s="25">
         <v>2828650496</v>
       </c>
-      <c r="K2" s="24">
+      <c r="L2" s="24">
         <v>31371</v>
       </c>
-      <c r="L2" s="24">
+      <c r="M2" s="24">
         <v>32571</v>
       </c>
-      <c r="M2" s="11">
+      <c r="N2" s="11">
         <v>0.4668</v>
       </c>
-      <c r="N2" s="11">
+      <c r="O2" s="11">
         <v>2.14</v>
       </c>
-      <c r="O2" s="28">
-        <f t="shared" ref="O2:O7" si="1">0.4668/M2</f>
+      <c r="P2" s="28">
+        <f t="shared" ref="P2:P7" si="1">0.4668/N2</f>
         <v>1</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>16.18</v>
       </c>
     </row>
-    <row r="3" ht="17.6" spans="1:16">
+    <row r="3" ht="17.6" spans="1:17">
       <c r="A3">
         <v>3</v>
       </c>
@@ -11066,45 +11072,48 @@
         <v>62.7</v>
       </c>
       <c r="E3" s="9">
+        <v>35.1</v>
+      </c>
+      <c r="F3" s="9">
         <v>39.8</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="9">
         <v>77.7</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="9">
         <v>73.6</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <f t="shared" si="0"/>
-        <v>57.05</v>
-      </c>
-      <c r="I3" s="14">
+        <v>53.9142857142857</v>
+      </c>
+      <c r="J3" s="14">
         <v>14714784320</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>2672936960</v>
       </c>
-      <c r="K3" s="14">
+      <c r="L3" s="14">
         <v>28203</v>
       </c>
-      <c r="L3" s="17">
+      <c r="M3" s="17">
         <v>29403</v>
       </c>
-      <c r="M3" s="17">
+      <c r="N3" s="17">
         <v>0.4094</v>
       </c>
-      <c r="N3" s="17">
+      <c r="O3" s="17">
         <v>2.44</v>
       </c>
-      <c r="O3" s="28">
+      <c r="P3" s="28">
         <f t="shared" si="1"/>
         <v>1.14020517830972</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>17.06</v>
       </c>
     </row>
-    <row r="4" ht="17.6" spans="1:16">
+    <row r="4" ht="17.6" spans="1:17">
       <c r="A4">
         <v>6</v>
       </c>
@@ -11118,45 +11127,48 @@
         <v>71.5</v>
       </c>
       <c r="E4" s="9">
+        <v>31.3</v>
+      </c>
+      <c r="F4" s="9">
         <v>42.6</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G4" s="9">
         <v>78.1</v>
       </c>
-      <c r="G4" s="9">
+      <c r="H4" s="9">
         <v>74</v>
       </c>
-      <c r="H4" s="15">
+      <c r="I4" s="15">
         <f t="shared" si="0"/>
-        <v>59.3</v>
-      </c>
-      <c r="I4" s="16">
+        <v>55.3</v>
+      </c>
+      <c r="J4" s="16">
         <v>13053840512</v>
       </c>
-      <c r="J4" s="12">
+      <c r="K4" s="12">
         <v>2517223424</v>
       </c>
-      <c r="K4" s="16">
+      <c r="L4" s="16">
         <v>25035</v>
       </c>
-      <c r="L4" s="18">
+      <c r="M4" s="18">
         <v>26235</v>
       </c>
-      <c r="M4" s="18">
+      <c r="N4" s="18">
         <v>0.374</v>
       </c>
-      <c r="N4" s="18">
+      <c r="O4" s="18">
         <v>2.67</v>
       </c>
-      <c r="O4" s="28">
+      <c r="P4" s="28">
         <f t="shared" si="1"/>
         <v>1.24812834224599</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>18.48</v>
       </c>
     </row>
-    <row r="5" ht="17.6" spans="1:16">
+    <row r="5" ht="17.6" spans="1:17">
       <c r="A5">
         <v>9</v>
       </c>
@@ -11170,45 +11182,48 @@
         <v>57.8</v>
       </c>
       <c r="E5" s="7">
+        <v>30.1</v>
+      </c>
+      <c r="F5" s="7">
         <v>41.2</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>74.2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>71.2</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="13">
         <f t="shared" si="0"/>
-        <v>58.3166666666667</v>
-      </c>
-      <c r="I5" s="14">
+        <v>54.2857142857143</v>
+      </c>
+      <c r="J5" s="14">
         <v>11392896704</v>
       </c>
-      <c r="J5" s="12">
+      <c r="K5" s="12">
         <v>2361509888</v>
       </c>
-      <c r="K5" s="14">
+      <c r="L5" s="14">
         <v>21868</v>
       </c>
-      <c r="L5" s="17">
+      <c r="M5" s="17">
         <v>23068</v>
       </c>
-      <c r="M5" s="17">
+      <c r="N5" s="17">
         <v>0.3372</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="17">
         <v>2.97</v>
       </c>
-      <c r="O5" s="28">
+      <c r="P5" s="28">
         <f t="shared" si="1"/>
         <v>1.38434163701068</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>20.37</v>
       </c>
     </row>
-    <row r="6" ht="17.6" spans="1:16">
+    <row r="6" ht="17.6" spans="1:17">
       <c r="A6">
         <v>12</v>
       </c>
@@ -11222,45 +11237,48 @@
         <v>57.9</v>
       </c>
       <c r="E6" s="9">
+        <v>28.5</v>
+      </c>
+      <c r="F6" s="9">
         <v>37.4</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>72.5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>70.3</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I6" s="15">
         <f t="shared" si="0"/>
-        <v>56.3</v>
-      </c>
-      <c r="I6" s="16">
+        <v>52.3285714285714</v>
+      </c>
+      <c r="J6" s="16">
         <v>9731952896</v>
       </c>
-      <c r="J6" s="12">
+      <c r="K6" s="12">
         <v>2205796352</v>
       </c>
-      <c r="K6" s="16">
+      <c r="L6" s="16">
         <v>18700</v>
       </c>
-      <c r="L6" s="18">
+      <c r="M6" s="18">
         <v>19900</v>
       </c>
-      <c r="M6" s="18">
+      <c r="N6" s="18">
         <v>0.2955</v>
       </c>
-      <c r="N6" s="18">
+      <c r="O6" s="18">
         <v>3.38</v>
       </c>
-      <c r="O6" s="28">
+      <c r="P6" s="28">
         <f t="shared" si="1"/>
         <v>1.57969543147208</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>20.62</v>
       </c>
     </row>
-    <row r="7" ht="17.6" spans="1:16">
+    <row r="7" ht="17.6" spans="1:17">
       <c r="A7">
         <v>15</v>
       </c>
@@ -11274,41 +11292,44 @@
         <v>55.6</v>
       </c>
       <c r="E7" s="7">
+        <v>25.3</v>
+      </c>
+      <c r="F7" s="7">
         <v>31.8</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>70.4</v>
       </c>
-      <c r="G7" s="7">
+      <c r="H7" s="7">
         <v>69.1</v>
       </c>
-      <c r="H7" s="13">
+      <c r="I7" s="13">
         <f t="shared" si="0"/>
-        <v>53.5166666666667</v>
-      </c>
-      <c r="I7" s="17">
+        <v>49.4857142857143</v>
+      </c>
+      <c r="J7" s="17">
         <v>8071009088</v>
       </c>
-      <c r="J7" s="12">
+      <c r="K7" s="12">
         <v>2050082816</v>
       </c>
-      <c r="K7" s="17">
+      <c r="L7" s="17">
         <v>15532</v>
       </c>
-      <c r="L7" s="17">
+      <c r="M7" s="17">
         <v>16732</v>
       </c>
-      <c r="M7" s="17">
+      <c r="N7" s="17">
         <v>0.2535</v>
       </c>
-      <c r="N7" s="17">
+      <c r="O7" s="17">
         <v>3.94</v>
       </c>
-      <c r="O7" s="28">
+      <c r="P7" s="28">
         <f t="shared" si="1"/>
         <v>1.8414201183432</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>22.77</v>
       </c>
     </row>
@@ -13176,811 +13197,6 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="B6:I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
-  <sheetData>
-    <row r="1" ht="17.6" spans="1:18">
-      <c r="A1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>170</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="R1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" ht="17.6" spans="1:18">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>48.3</v>
-      </c>
-      <c r="C2" s="6">
-        <v>72.7</v>
-      </c>
-      <c r="D2" s="6">
-        <v>77.4</v>
-      </c>
-      <c r="E2" s="6">
-        <v>38.3</v>
-      </c>
-      <c r="F2" s="6">
-        <v>44.2</v>
-      </c>
-      <c r="G2" s="6">
-        <v>78.7</v>
-      </c>
-      <c r="H2" s="6">
-        <v>63.2</v>
-      </c>
-      <c r="I2" s="6">
-        <v>70.1</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
-        <v>61.6125</v>
-      </c>
-      <c r="K2" s="24">
-        <v>16375728128</v>
-      </c>
-      <c r="L2" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M2" s="24">
-        <v>31371</v>
-      </c>
-      <c r="N2" s="24">
-        <v>32571</v>
-      </c>
-      <c r="O2" s="11">
-        <v>0.4668</v>
-      </c>
-      <c r="P2" s="11">
-        <v>2.14</v>
-      </c>
-      <c r="Q2" s="28">
-        <f t="shared" ref="Q2:Q7" si="1">0.4884/O2</f>
-        <v>1.04627249357326</v>
-      </c>
-      <c r="R2">
-        <v>16.18</v>
-      </c>
-    </row>
-    <row r="3" ht="17.6" spans="1:18">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7">
-        <v>43.2</v>
-      </c>
-      <c r="C3" s="7">
-        <v>73.9</v>
-      </c>
-      <c r="D3" s="7">
-        <v>73</v>
-      </c>
-      <c r="E3" s="7">
-        <v>35.4</v>
-      </c>
-      <c r="F3" s="7">
-        <v>41.2</v>
-      </c>
-      <c r="G3" s="7">
-        <v>78.2</v>
-      </c>
-      <c r="H3" s="7">
-        <v>61.7</v>
-      </c>
-      <c r="I3" s="7">
-        <v>69.5</v>
-      </c>
-      <c r="J3" s="13">
-        <f t="shared" si="0"/>
-        <v>59.5125</v>
-      </c>
-      <c r="K3" s="26">
-        <v>14870497802</v>
-      </c>
-      <c r="L3" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M3" s="26">
-        <v>28500</v>
-      </c>
-      <c r="N3" s="26">
-        <v>29700</v>
-      </c>
-      <c r="O3" s="26">
-        <v>0.4208</v>
-      </c>
-      <c r="P3" s="26">
-        <v>2.38</v>
-      </c>
-      <c r="Q3" s="28">
-        <f t="shared" si="1"/>
-        <v>1.1606463878327</v>
-      </c>
-      <c r="R3">
-        <v>16.56</v>
-      </c>
-    </row>
-    <row r="4" ht="17.6" spans="1:18">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4" s="9">
-        <v>38.7</v>
-      </c>
-      <c r="C4" s="9">
-        <v>71.8</v>
-      </c>
-      <c r="D4" s="9">
-        <v>67.2</v>
-      </c>
-      <c r="E4" s="9">
-        <v>31.6</v>
-      </c>
-      <c r="F4" s="9">
-        <v>37.4</v>
-      </c>
-      <c r="G4" s="9">
-        <v>77</v>
-      </c>
-      <c r="H4" s="9">
-        <v>61.4</v>
-      </c>
-      <c r="I4" s="9">
-        <v>66.5</v>
-      </c>
-      <c r="J4" s="15">
-        <f t="shared" si="0"/>
-        <v>56.45</v>
-      </c>
-      <c r="K4" s="27">
-        <v>13365267476</v>
-      </c>
-      <c r="L4" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M4" s="27">
-        <v>25629</v>
-      </c>
-      <c r="N4" s="27">
-        <v>26289</v>
-      </c>
-      <c r="O4" s="27">
-        <v>0.4043</v>
-      </c>
-      <c r="P4" s="27">
-        <v>2.47</v>
-      </c>
-      <c r="Q4" s="28">
-        <f t="shared" si="1"/>
-        <v>1.20801385110067</v>
-      </c>
-      <c r="R4">
-        <v>16.79</v>
-      </c>
-    </row>
-    <row r="5" ht="17.6" spans="1:18">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7">
-        <v>37.9</v>
-      </c>
-      <c r="C5" s="7">
-        <v>72.3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>64.4</v>
-      </c>
-      <c r="E5" s="7">
-        <v>27.1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>37.6</v>
-      </c>
-      <c r="G5" s="7">
-        <v>75.9</v>
-      </c>
-      <c r="H5" s="7">
-        <v>61.7</v>
-      </c>
-      <c r="I5" s="7">
-        <v>67</v>
-      </c>
-      <c r="J5" s="13">
-        <f t="shared" si="0"/>
-        <v>55.4875</v>
-      </c>
-      <c r="K5" s="26">
-        <v>11860037150</v>
-      </c>
-      <c r="L5" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M5" s="26">
-        <v>22759</v>
-      </c>
-      <c r="N5" s="26">
-        <v>23958</v>
-      </c>
-      <c r="O5" s="26">
-        <v>0.3755</v>
-      </c>
-      <c r="P5" s="26">
-        <v>2.66</v>
-      </c>
-      <c r="Q5" s="28">
-        <f t="shared" si="1"/>
-        <v>1.30066577896138</v>
-      </c>
-      <c r="R5">
-        <v>17.11</v>
-      </c>
-    </row>
-    <row r="6" ht="17.6" spans="1:18">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9">
-        <v>34.5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>69.8</v>
-      </c>
-      <c r="D6" s="9">
-        <v>59.4</v>
-      </c>
-      <c r="E6" s="9">
-        <v>24.1</v>
-      </c>
-      <c r="F6" s="9">
-        <v>33.8</v>
-      </c>
-      <c r="G6" s="9">
-        <v>73.4</v>
-      </c>
-      <c r="H6" s="9">
-        <v>61.5</v>
-      </c>
-      <c r="I6" s="9">
-        <v>65.5</v>
-      </c>
-      <c r="J6" s="15">
-        <f t="shared" si="0"/>
-        <v>52.75</v>
-      </c>
-      <c r="K6" s="27">
-        <v>10354806824</v>
-      </c>
-      <c r="L6" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M6" s="27">
-        <v>19888</v>
-      </c>
-      <c r="N6" s="27">
-        <v>21088</v>
-      </c>
-      <c r="O6" s="27">
-        <v>0.3246</v>
-      </c>
-      <c r="P6" s="27">
-        <v>3.08</v>
-      </c>
-      <c r="Q6" s="28">
-        <f t="shared" si="1"/>
-        <v>1.50462107208872</v>
-      </c>
-      <c r="R6">
-        <v>17.76</v>
-      </c>
-    </row>
-    <row r="7" ht="17.6" spans="1:18">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7">
-        <v>30.4</v>
-      </c>
-      <c r="C7" s="7">
-        <v>65.5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>52</v>
-      </c>
-      <c r="E7" s="7">
-        <v>24</v>
-      </c>
-      <c r="F7" s="7">
-        <v>31.4</v>
-      </c>
-      <c r="G7" s="7">
-        <v>68.7</v>
-      </c>
-      <c r="H7" s="7">
-        <v>56</v>
-      </c>
-      <c r="I7" s="7">
-        <v>63.8</v>
-      </c>
-      <c r="J7" s="13">
-        <f t="shared" si="0"/>
-        <v>48.975</v>
-      </c>
-      <c r="K7" s="26">
-        <v>8849576498</v>
-      </c>
-      <c r="L7" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="M7" s="26">
-        <v>17017</v>
-      </c>
-      <c r="N7" s="26">
-        <v>18217</v>
-      </c>
-      <c r="O7" s="26">
-        <v>0.295</v>
-      </c>
-      <c r="P7" s="26">
-        <v>3.39</v>
-      </c>
-      <c r="Q7" s="28">
-        <f t="shared" si="1"/>
-        <v>1.65559322033898</v>
-      </c>
-      <c r="R7">
-        <v>18.68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:P7"/>
-  <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
-  <cols>
-    <col min="9" max="9" width="12.9230769230769"/>
-    <col min="10" max="10" width="10"/>
-    <col min="15" max="15" width="12.9230769230769"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="17.6" spans="1:16">
-      <c r="A1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="P1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" ht="17.6" spans="1:16">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>48.3</v>
-      </c>
-      <c r="C2" s="6">
-        <v>72.7</v>
-      </c>
-      <c r="D2" s="6">
-        <v>77.4</v>
-      </c>
-      <c r="E2" s="6">
-        <v>44.2</v>
-      </c>
-      <c r="F2" s="6">
-        <v>78.7</v>
-      </c>
-      <c r="G2" s="6">
-        <v>70.1</v>
-      </c>
-      <c r="H2" s="3">
-        <f t="shared" ref="H2:H7" si="0">AVERAGE(B2:G2)</f>
-        <v>65.2333333333333</v>
-      </c>
-      <c r="I2" s="24">
-        <v>16375728128</v>
-      </c>
-      <c r="J2" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K2" s="24">
-        <v>31371</v>
-      </c>
-      <c r="L2" s="24">
-        <v>32571</v>
-      </c>
-      <c r="M2" s="11">
-        <v>0.4668</v>
-      </c>
-      <c r="N2" s="11">
-        <v>2.14</v>
-      </c>
-      <c r="O2" s="28">
-        <f t="shared" ref="O2:O7" si="1">0.4668/M2</f>
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>16.18</v>
-      </c>
-    </row>
-    <row r="3" ht="17.6" spans="1:16">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="7">
-        <v>45.4</v>
-      </c>
-      <c r="C3" s="7">
-        <v>74.1</v>
-      </c>
-      <c r="D3" s="7">
-        <v>75.8</v>
-      </c>
-      <c r="E3" s="7">
-        <v>41.8</v>
-      </c>
-      <c r="F3" s="7">
-        <v>79.7</v>
-      </c>
-      <c r="G3" s="7">
-        <v>71.5</v>
-      </c>
-      <c r="H3" s="15">
-        <f t="shared" si="0"/>
-        <v>64.7166666666667</v>
-      </c>
-      <c r="I3" s="26">
-        <v>14870497802</v>
-      </c>
-      <c r="J3" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K3" s="26">
-        <v>28500</v>
-      </c>
-      <c r="L3" s="26">
-        <v>29700</v>
-      </c>
-      <c r="M3" s="26">
-        <v>0.4208</v>
-      </c>
-      <c r="N3" s="26">
-        <v>2.38</v>
-      </c>
-      <c r="O3" s="28">
-        <f t="shared" si="1"/>
-        <v>1.10931558935361</v>
-      </c>
-      <c r="P3">
-        <v>16.56</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:16">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7">
-        <v>45.9</v>
-      </c>
-      <c r="C4" s="7">
-        <v>75.1</v>
-      </c>
-      <c r="D4" s="7">
-        <v>75</v>
-      </c>
-      <c r="E4" s="7">
-        <v>42.4</v>
-      </c>
-      <c r="F4" s="7">
-        <v>79.4</v>
-      </c>
-      <c r="G4" s="7">
-        <v>74.7</v>
-      </c>
-      <c r="H4" s="15">
-        <f t="shared" si="0"/>
-        <v>65.4166666666667</v>
-      </c>
-      <c r="I4" s="27">
-        <v>13365267476</v>
-      </c>
-      <c r="J4" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K4" s="27">
-        <v>25629</v>
-      </c>
-      <c r="L4" s="27">
-        <v>26289</v>
-      </c>
-      <c r="M4" s="27">
-        <v>0.4043</v>
-      </c>
-      <c r="N4" s="27">
-        <v>2.47</v>
-      </c>
-      <c r="O4" s="28">
-        <f t="shared" si="1"/>
-        <v>1.15458817709622</v>
-      </c>
-      <c r="P4">
-        <v>16.79</v>
-      </c>
-    </row>
-    <row r="5" ht="17.6" spans="1:16">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7">
-        <v>43.5</v>
-      </c>
-      <c r="C5" s="7">
-        <v>76.7</v>
-      </c>
-      <c r="D5" s="7">
-        <v>69</v>
-      </c>
-      <c r="E5" s="7">
-        <v>38.6</v>
-      </c>
-      <c r="F5" s="7">
-        <v>77.4</v>
-      </c>
-      <c r="G5" s="7">
-        <v>73.6</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>63.1333333333333</v>
-      </c>
-      <c r="I5" s="26">
-        <v>11860037150</v>
-      </c>
-      <c r="J5" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K5" s="26">
-        <v>22759</v>
-      </c>
-      <c r="L5" s="26">
-        <v>23958</v>
-      </c>
-      <c r="M5" s="26">
-        <v>0.3755</v>
-      </c>
-      <c r="N5" s="26">
-        <v>2.66</v>
-      </c>
-      <c r="O5" s="28">
-        <f t="shared" si="1"/>
-        <v>1.24314247669774</v>
-      </c>
-      <c r="P5">
-        <v>17.11</v>
-      </c>
-    </row>
-    <row r="6" ht="17.6" spans="1:16">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6" s="9">
-        <v>36.1</v>
-      </c>
-      <c r="C6" s="9">
-        <v>77.5</v>
-      </c>
-      <c r="D6" s="9">
-        <v>63</v>
-      </c>
-      <c r="E6" s="9">
-        <v>35.4</v>
-      </c>
-      <c r="F6" s="9">
-        <v>73.7</v>
-      </c>
-      <c r="G6" s="9">
-        <v>69.7</v>
-      </c>
-      <c r="H6" s="15">
-        <f t="shared" si="0"/>
-        <v>59.2333333333333</v>
-      </c>
-      <c r="I6" s="27">
-        <v>10354806824</v>
-      </c>
-      <c r="J6" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K6" s="27">
-        <v>19888</v>
-      </c>
-      <c r="L6" s="27">
-        <v>21088</v>
-      </c>
-      <c r="M6" s="27">
-        <v>0.3246</v>
-      </c>
-      <c r="N6" s="27">
-        <v>3.08</v>
-      </c>
-      <c r="O6" s="28">
-        <f t="shared" si="1"/>
-        <v>1.43807763401109</v>
-      </c>
-      <c r="P6">
-        <v>17.76</v>
-      </c>
-    </row>
-    <row r="7" ht="17.6" spans="1:16">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" s="7">
-        <v>35.5</v>
-      </c>
-      <c r="C7" s="7">
-        <v>72.3</v>
-      </c>
-      <c r="D7" s="7">
-        <v>58.9</v>
-      </c>
-      <c r="E7" s="7">
-        <v>35.2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>73.3</v>
-      </c>
-      <c r="G7" s="7">
-        <v>71</v>
-      </c>
-      <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>57.7</v>
-      </c>
-      <c r="I7" s="26">
-        <v>8849576498</v>
-      </c>
-      <c r="J7" s="25">
-        <v>2828650496</v>
-      </c>
-      <c r="K7" s="26">
-        <v>17017</v>
-      </c>
-      <c r="L7" s="26">
-        <v>18217</v>
-      </c>
-      <c r="M7" s="26">
-        <v>0.295</v>
-      </c>
-      <c r="N7" s="26">
-        <v>3.39</v>
-      </c>
-      <c r="O7" s="28">
-        <f t="shared" si="1"/>
-        <v>1.58237288135593</v>
-      </c>
-      <c r="P7">
-        <v>18.68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:R7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -14391,6 +13607,832 @@
       <c r="Q7" s="28">
         <f t="shared" si="0"/>
         <v>1.58237288135593</v>
+      </c>
+      <c r="R7">
+        <v>18.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <cols>
+    <col min="10" max="10" width="12.9230769230769"/>
+    <col min="11" max="11" width="10"/>
+    <col min="16" max="16" width="12.9230769230769"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="17.6" spans="1:17">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" ht="17.6" spans="1:17">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>48.3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>72.7</v>
+      </c>
+      <c r="D2" s="6">
+        <v>77.4</v>
+      </c>
+      <c r="E2" s="6">
+        <v>38.3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>44.2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>78.7</v>
+      </c>
+      <c r="H2" s="6">
+        <v>70.1</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I7" si="0">AVERAGE(B2:H2)</f>
+        <v>61.3857142857143</v>
+      </c>
+      <c r="J2" s="24">
+        <v>16375728128</v>
+      </c>
+      <c r="K2" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L2" s="24">
+        <v>31371</v>
+      </c>
+      <c r="M2" s="24">
+        <v>32571</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0.4668</v>
+      </c>
+      <c r="O2" s="11">
+        <v>2.14</v>
+      </c>
+      <c r="P2" s="28">
+        <f t="shared" ref="P2:P7" si="1">0.4668/N2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="3" ht="17.6" spans="1:17">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7">
+        <v>45.4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>74.1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>75.8</v>
+      </c>
+      <c r="E3" s="7">
+        <v>40.4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>41.8</v>
+      </c>
+      <c r="G3" s="7">
+        <v>79.7</v>
+      </c>
+      <c r="H3" s="7">
+        <v>71.5</v>
+      </c>
+      <c r="I3" s="15">
+        <f t="shared" si="0"/>
+        <v>61.2428571428571</v>
+      </c>
+      <c r="J3" s="26">
+        <v>14870497802</v>
+      </c>
+      <c r="K3" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L3" s="26">
+        <v>28500</v>
+      </c>
+      <c r="M3" s="26">
+        <v>29700</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0.4208</v>
+      </c>
+      <c r="O3" s="26">
+        <v>2.38</v>
+      </c>
+      <c r="P3" s="28">
+        <f t="shared" si="1"/>
+        <v>1.10931558935361</v>
+      </c>
+      <c r="Q3">
+        <v>16.56</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:17">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7">
+        <v>45.9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>75.1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>75</v>
+      </c>
+      <c r="E4" s="7">
+        <v>31.4</v>
+      </c>
+      <c r="F4" s="7">
+        <v>42.4</v>
+      </c>
+      <c r="G4" s="7">
+        <v>79.4</v>
+      </c>
+      <c r="H4" s="7">
+        <v>74.7</v>
+      </c>
+      <c r="I4" s="15">
+        <f t="shared" si="0"/>
+        <v>60.5571428571429</v>
+      </c>
+      <c r="J4" s="27">
+        <v>13365267476</v>
+      </c>
+      <c r="K4" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L4" s="27">
+        <v>25629</v>
+      </c>
+      <c r="M4" s="27">
+        <v>26289</v>
+      </c>
+      <c r="N4" s="27">
+        <v>0.4043</v>
+      </c>
+      <c r="O4" s="27">
+        <v>2.47</v>
+      </c>
+      <c r="P4" s="28">
+        <f t="shared" si="1"/>
+        <v>1.15458817709622</v>
+      </c>
+      <c r="Q4">
+        <v>16.79</v>
+      </c>
+    </row>
+    <row r="5" ht="17.6" spans="1:17">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7">
+        <v>43.5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>76.7</v>
+      </c>
+      <c r="D5" s="7">
+        <v>69</v>
+      </c>
+      <c r="E5" s="7">
+        <v>29.1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>38.6</v>
+      </c>
+      <c r="G5" s="7">
+        <v>77.4</v>
+      </c>
+      <c r="H5" s="7">
+        <v>73.6</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>58.2714285714286</v>
+      </c>
+      <c r="J5" s="26">
+        <v>11860037150</v>
+      </c>
+      <c r="K5" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L5" s="26">
+        <v>22759</v>
+      </c>
+      <c r="M5" s="26">
+        <v>23958</v>
+      </c>
+      <c r="N5" s="26">
+        <v>0.3755</v>
+      </c>
+      <c r="O5" s="26">
+        <v>2.66</v>
+      </c>
+      <c r="P5" s="28">
+        <f t="shared" si="1"/>
+        <v>1.24314247669774</v>
+      </c>
+      <c r="Q5">
+        <v>17.11</v>
+      </c>
+    </row>
+    <row r="6" ht="17.6" spans="1:17">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>36.1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>77.5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>63</v>
+      </c>
+      <c r="E6" s="9">
+        <v>25.4</v>
+      </c>
+      <c r="F6" s="9">
+        <v>35.4</v>
+      </c>
+      <c r="G6" s="9">
+        <v>73.7</v>
+      </c>
+      <c r="H6" s="9">
+        <v>69.7</v>
+      </c>
+      <c r="I6" s="15">
+        <f t="shared" si="0"/>
+        <v>54.4</v>
+      </c>
+      <c r="J6" s="27">
+        <v>10354806824</v>
+      </c>
+      <c r="K6" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L6" s="27">
+        <v>19888</v>
+      </c>
+      <c r="M6" s="27">
+        <v>21088</v>
+      </c>
+      <c r="N6" s="27">
+        <v>0.3246</v>
+      </c>
+      <c r="O6" s="27">
+        <v>3.08</v>
+      </c>
+      <c r="P6" s="28">
+        <f t="shared" si="1"/>
+        <v>1.43807763401109</v>
+      </c>
+      <c r="Q6">
+        <v>17.76</v>
+      </c>
+    </row>
+    <row r="7" ht="17.6" spans="1:17">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7">
+        <v>35.5</v>
+      </c>
+      <c r="C7" s="7">
+        <v>72.3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>58.9</v>
+      </c>
+      <c r="E7" s="7">
+        <v>24.5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>35.2</v>
+      </c>
+      <c r="G7" s="7">
+        <v>73.3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>71</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>52.9571428571429</v>
+      </c>
+      <c r="J7" s="26">
+        <v>8849576498</v>
+      </c>
+      <c r="K7" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="L7" s="26">
+        <v>17017</v>
+      </c>
+      <c r="M7" s="26">
+        <v>18217</v>
+      </c>
+      <c r="N7" s="26">
+        <v>0.295</v>
+      </c>
+      <c r="O7" s="26">
+        <v>3.39</v>
+      </c>
+      <c r="P7" s="28">
+        <f t="shared" si="1"/>
+        <v>1.58237288135593</v>
+      </c>
+      <c r="Q7">
+        <v>18.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="B6:I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <sheetData>
+    <row r="1" ht="17.6" spans="1:18">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K1" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" ht="17.6" spans="1:18">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>48.3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>72.7</v>
+      </c>
+      <c r="D2" s="6">
+        <v>77.4</v>
+      </c>
+      <c r="E2" s="6">
+        <v>38.3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>44.2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>78.7</v>
+      </c>
+      <c r="H2" s="6">
+        <v>63.2</v>
+      </c>
+      <c r="I2" s="6">
+        <v>70.1</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J7" si="0">AVERAGE(B2:I2)</f>
+        <v>61.6125</v>
+      </c>
+      <c r="K2" s="24">
+        <v>16375728128</v>
+      </c>
+      <c r="L2" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M2" s="24">
+        <v>31371</v>
+      </c>
+      <c r="N2" s="24">
+        <v>32571</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0.4668</v>
+      </c>
+      <c r="P2" s="11">
+        <v>2.14</v>
+      </c>
+      <c r="Q2" s="28">
+        <f t="shared" ref="Q2:Q7" si="1">0.4884/O2</f>
+        <v>1.04627249357326</v>
+      </c>
+      <c r="R2">
+        <v>16.18</v>
+      </c>
+    </row>
+    <row r="3" ht="17.6" spans="1:18">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7">
+        <v>43.2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>73.9</v>
+      </c>
+      <c r="D3" s="7">
+        <v>73</v>
+      </c>
+      <c r="E3" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="F3" s="7">
+        <v>41.2</v>
+      </c>
+      <c r="G3" s="7">
+        <v>78.2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>61.7</v>
+      </c>
+      <c r="I3" s="7">
+        <v>69.5</v>
+      </c>
+      <c r="J3" s="13">
+        <f t="shared" si="0"/>
+        <v>59.5125</v>
+      </c>
+      <c r="K3" s="26">
+        <v>14870497802</v>
+      </c>
+      <c r="L3" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M3" s="26">
+        <v>28500</v>
+      </c>
+      <c r="N3" s="26">
+        <v>29700</v>
+      </c>
+      <c r="O3" s="26">
+        <v>0.4208</v>
+      </c>
+      <c r="P3" s="26">
+        <v>2.38</v>
+      </c>
+      <c r="Q3" s="28">
+        <f t="shared" si="1"/>
+        <v>1.1606463878327</v>
+      </c>
+      <c r="R3">
+        <v>16.56</v>
+      </c>
+    </row>
+    <row r="4" ht="17.6" spans="1:18">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>38.7</v>
+      </c>
+      <c r="C4" s="9">
+        <v>71.8</v>
+      </c>
+      <c r="D4" s="9">
+        <v>67.2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>31.6</v>
+      </c>
+      <c r="F4" s="9">
+        <v>37.4</v>
+      </c>
+      <c r="G4" s="9">
+        <v>77</v>
+      </c>
+      <c r="H4" s="9">
+        <v>61.4</v>
+      </c>
+      <c r="I4" s="9">
+        <v>66.5</v>
+      </c>
+      <c r="J4" s="15">
+        <f t="shared" si="0"/>
+        <v>56.45</v>
+      </c>
+      <c r="K4" s="27">
+        <v>13365267476</v>
+      </c>
+      <c r="L4" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M4" s="27">
+        <v>25629</v>
+      </c>
+      <c r="N4" s="27">
+        <v>26289</v>
+      </c>
+      <c r="O4" s="27">
+        <v>0.4043</v>
+      </c>
+      <c r="P4" s="27">
+        <v>2.47</v>
+      </c>
+      <c r="Q4" s="28">
+        <f t="shared" si="1"/>
+        <v>1.20801385110067</v>
+      </c>
+      <c r="R4">
+        <v>16.79</v>
+      </c>
+    </row>
+    <row r="5" ht="17.6" spans="1:18">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7">
+        <v>37.9</v>
+      </c>
+      <c r="C5" s="7">
+        <v>72.3</v>
+      </c>
+      <c r="D5" s="7">
+        <v>64.4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>27.1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>37.6</v>
+      </c>
+      <c r="G5" s="7">
+        <v>75.9</v>
+      </c>
+      <c r="H5" s="7">
+        <v>61.7</v>
+      </c>
+      <c r="I5" s="7">
+        <v>67</v>
+      </c>
+      <c r="J5" s="13">
+        <f t="shared" si="0"/>
+        <v>55.4875</v>
+      </c>
+      <c r="K5" s="26">
+        <v>11860037150</v>
+      </c>
+      <c r="L5" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M5" s="26">
+        <v>22759</v>
+      </c>
+      <c r="N5" s="26">
+        <v>23958</v>
+      </c>
+      <c r="O5" s="26">
+        <v>0.3755</v>
+      </c>
+      <c r="P5" s="26">
+        <v>2.66</v>
+      </c>
+      <c r="Q5" s="28">
+        <f t="shared" si="1"/>
+        <v>1.30066577896138</v>
+      </c>
+      <c r="R5">
+        <v>17.11</v>
+      </c>
+    </row>
+    <row r="6" ht="17.6" spans="1:18">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>34.5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>69.8</v>
+      </c>
+      <c r="D6" s="9">
+        <v>59.4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>24.1</v>
+      </c>
+      <c r="F6" s="9">
+        <v>33.8</v>
+      </c>
+      <c r="G6" s="9">
+        <v>73.4</v>
+      </c>
+      <c r="H6" s="9">
+        <v>61.5</v>
+      </c>
+      <c r="I6" s="9">
+        <v>65.5</v>
+      </c>
+      <c r="J6" s="15">
+        <f t="shared" si="0"/>
+        <v>52.75</v>
+      </c>
+      <c r="K6" s="27">
+        <v>10354806824</v>
+      </c>
+      <c r="L6" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M6" s="27">
+        <v>19888</v>
+      </c>
+      <c r="N6" s="27">
+        <v>21088</v>
+      </c>
+      <c r="O6" s="27">
+        <v>0.3246</v>
+      </c>
+      <c r="P6" s="27">
+        <v>3.08</v>
+      </c>
+      <c r="Q6" s="28">
+        <f t="shared" si="1"/>
+        <v>1.50462107208872</v>
+      </c>
+      <c r="R6">
+        <v>17.76</v>
+      </c>
+    </row>
+    <row r="7" ht="17.6" spans="1:18">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7">
+        <v>30.4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>65.5</v>
+      </c>
+      <c r="D7" s="7">
+        <v>52</v>
+      </c>
+      <c r="E7" s="7">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7">
+        <v>31.4</v>
+      </c>
+      <c r="G7" s="7">
+        <v>68.7</v>
+      </c>
+      <c r="H7" s="7">
+        <v>56</v>
+      </c>
+      <c r="I7" s="7">
+        <v>63.8</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" si="0"/>
+        <v>48.975</v>
+      </c>
+      <c r="K7" s="26">
+        <v>8849576498</v>
+      </c>
+      <c r="L7" s="25">
+        <v>2828650496</v>
+      </c>
+      <c r="M7" s="26">
+        <v>17017</v>
+      </c>
+      <c r="N7" s="26">
+        <v>18217</v>
+      </c>
+      <c r="O7" s="26">
+        <v>0.295</v>
+      </c>
+      <c r="P7" s="26">
+        <v>3.39</v>
+      </c>
+      <c r="Q7" s="28">
+        <f t="shared" si="1"/>
+        <v>1.65559322033898</v>
       </c>
       <c r="R7">
         <v>18.68</v>

</xml_diff>

<commit_message>
add: condor eval dataset
</commit_message>
<xml_diff>
--- a/moe_prune/ppl_result.xlsx
+++ b/moe_prune/ppl_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9500" tabRatio="872" firstSheet="31" activeTab="39"/>
+    <workbookView windowWidth="25600" windowHeight="9500" tabRatio="872" firstSheet="15" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="193">
   <si>
     <t>origin PPL</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>ppl</t>
+  </si>
+  <si>
+    <t>js</t>
   </si>
 </sst>
 </file>
@@ -13144,8 +13147,8 @@
   <sheetPr/>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7"/>
@@ -20942,15 +20945,15 @@
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>126</v>
       </c>
@@ -20978,8 +20981,11 @@
       <c r="I1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -21008,8 +21014,11 @@
       <c r="I2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>0.165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -21027,8 +21036,11 @@
       <c r="I3">
         <v>12.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>0.022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -21046,8 +21058,11 @@
       <c r="I4">
         <v>12.07</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -21065,8 +21080,11 @@
       <c r="I5">
         <v>12.07</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>0.0194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -21084,8 +21102,11 @@
       <c r="I6">
         <v>12.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -21103,8 +21124,11 @@
       <c r="I7">
         <v>11.94</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -21122,8 +21146,11 @@
       <c r="I8">
         <v>11.89</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>0.0137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -21152,8 +21179,11 @@
       <c r="I9">
         <v>11.89</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>0.0141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -21171,8 +21201,11 @@
       <c r="I10">
         <v>12.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>0.0184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -21190,8 +21223,11 @@
       <c r="I11">
         <v>11.88</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>0.0144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -21209,8 +21245,11 @@
       <c r="I12">
         <v>11.87</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>0.0137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -21228,8 +21267,11 @@
       <c r="I13">
         <v>12.46</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>0.0188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -21258,8 +21300,11 @@
       <c r="I14">
         <v>11.91</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>0.0141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -21277,8 +21322,11 @@
       <c r="I15">
         <v>12.57</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>0.0197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -21296,8 +21344,11 @@
       <c r="I16">
         <v>11.96</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>0.0143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -21315,8 +21366,11 @@
       <c r="I17">
         <v>11.97</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>0.0129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -21334,8 +21388,11 @@
       <c r="I18">
         <v>12.43</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>0.0197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -21353,8 +21410,11 @@
       <c r="I19">
         <v>12.02</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19">
+        <v>0.0161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -21372,8 +21432,11 @@
       <c r="I20">
         <v>12.02</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20">
+        <v>0.0139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -21402,8 +21465,11 @@
       <c r="I21">
         <v>11.94</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>0.0131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -21432,8 +21498,11 @@
       <c r="I22">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22">
+        <v>0.0194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -21451,8 +21520,11 @@
       <c r="I23">
         <v>12.09</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23">
+        <v>0.0168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -21481,8 +21553,11 @@
       <c r="I24">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24">
+        <v>0.0141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -21511,8 +21586,11 @@
       <c r="I25">
         <v>11.98</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25">
+        <v>0.0196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -21530,8 +21608,11 @@
       <c r="I26">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>0.0404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -21549,8 +21630,11 @@
       <c r="I27">
         <v>12.73</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27">
+        <v>0.0665</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -21578,6 +21662,9 @@
       </c>
       <c r="I28">
         <v>12.85</v>
+      </c>
+      <c r="J28">
+        <v>0.0253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>